<commit_message>
-- Ajout Resultat du Test Kalman (5 essais)
</commit_message>
<xml_diff>
--- a/source/test/resultTestKalman.xlsx
+++ b/source/test/resultTestKalman.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>Step</t>
   </si>
@@ -34,6 +34,15 @@
   </si>
   <si>
     <t>VitesseTrue</t>
+  </si>
+  <si>
+    <t>KalmanGain</t>
+  </si>
+  <si>
+    <t>Confiance au système P</t>
+  </si>
+  <si>
+    <t>P</t>
   </si>
 </sst>
 </file>
@@ -517,8 +526,9 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" xfId="8"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -578,6 +588,895 @@
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>resultTest!$F$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>KalmanGain</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>resultTest!$A$2:$A$101</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="100"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>19</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>21</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>22</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>23</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>26</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>27</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>28</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>29</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>31</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>33</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>34</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>35</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>36</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>37</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>38</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>39</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>41</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>42</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>43</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>44</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>45</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>46</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>47</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>48</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>49</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>51</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>52</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>53</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>54</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>55</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>56</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>57</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>58</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>59</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>61</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>62</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>63</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>65</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>66</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>67</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>68</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>69</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>70</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>71</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>72</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>73</c:v>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v>74</c:v>
+                </c:pt>
+                <c:pt idx="75">
+                  <c:v>75</c:v>
+                </c:pt>
+                <c:pt idx="76">
+                  <c:v>76</c:v>
+                </c:pt>
+                <c:pt idx="77">
+                  <c:v>77</c:v>
+                </c:pt>
+                <c:pt idx="78">
+                  <c:v>78</c:v>
+                </c:pt>
+                <c:pt idx="79">
+                  <c:v>79</c:v>
+                </c:pt>
+                <c:pt idx="80">
+                  <c:v>80</c:v>
+                </c:pt>
+                <c:pt idx="81">
+                  <c:v>81</c:v>
+                </c:pt>
+                <c:pt idx="82">
+                  <c:v>82</c:v>
+                </c:pt>
+                <c:pt idx="83">
+                  <c:v>83</c:v>
+                </c:pt>
+                <c:pt idx="84">
+                  <c:v>84</c:v>
+                </c:pt>
+                <c:pt idx="85">
+                  <c:v>85</c:v>
+                </c:pt>
+                <c:pt idx="86">
+                  <c:v>86</c:v>
+                </c:pt>
+                <c:pt idx="87">
+                  <c:v>87</c:v>
+                </c:pt>
+                <c:pt idx="88">
+                  <c:v>88</c:v>
+                </c:pt>
+                <c:pt idx="89">
+                  <c:v>89</c:v>
+                </c:pt>
+                <c:pt idx="90">
+                  <c:v>90</c:v>
+                </c:pt>
+                <c:pt idx="91">
+                  <c:v>91</c:v>
+                </c:pt>
+                <c:pt idx="92">
+                  <c:v>92</c:v>
+                </c:pt>
+                <c:pt idx="93">
+                  <c:v>93</c:v>
+                </c:pt>
+                <c:pt idx="94">
+                  <c:v>94</c:v>
+                </c:pt>
+                <c:pt idx="95">
+                  <c:v>95</c:v>
+                </c:pt>
+                <c:pt idx="96">
+                  <c:v>96</c:v>
+                </c:pt>
+                <c:pt idx="97">
+                  <c:v>97</c:v>
+                </c:pt>
+                <c:pt idx="98">
+                  <c:v>98</c:v>
+                </c:pt>
+                <c:pt idx="99">
+                  <c:v>99</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>resultTest!$F$2:$F$101</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="100"/>
+                <c:pt idx="0">
+                  <c:v>2.0400299999999998</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.4293100000000001</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.1956199999999999</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.09382</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.0470900000000001</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.0262100000000001</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.0192399999999999</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1.0223899999999999</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1.0381400000000001</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1.07914</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1.18232</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1.4361600000000001</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1.9472100000000001</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>2.3772600000000002</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>1.7273400000000001</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>1.45112</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>1.6919</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>1.9096599999999999</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>1.5149999999999999</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>3.6111800000000001</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>3.2484299999999999</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>1.81172</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>1.36181</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>1.19096</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>1.1247499999999999</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>1.10076</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>1.08213</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>1.04671</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>1.0276000000000001</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>1.0188299999999999</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>1.0133399999999999</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>1.0102599999999999</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>1.00824</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>1.00688</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>1.00589</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>1.0051399999999999</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>1.0045299999999999</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>1.00404</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>1.00362</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>1.00326</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>1.00295</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>1.00268</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>1.00244</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>1.00223</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>1.0020500000000001</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>1.0018800000000001</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>1.00173</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>1.0016</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>1.0014799999999999</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>1.0013700000000001</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>1.0012700000000001</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>1.0011699999999999</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>1.00109</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>1.00101</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>1.00095</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>1.00088</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>1.00082</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>1.0007699999999999</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>1.0007200000000001</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>1.0006699999999999</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>1.0006299999999999</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>1.0005900000000001</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>1.0005500000000001</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>1.0005200000000001</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>1.00048</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>1.0004500000000001</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>1.0004200000000001</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>1.0004</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>1.00037</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>1.0003500000000001</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>1.0003299999999999</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>1.00031</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>1.0002899999999999</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>1.00027</c:v>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v>1.0002500000000001</c:v>
+                </c:pt>
+                <c:pt idx="75">
+                  <c:v>1.00024</c:v>
+                </c:pt>
+                <c:pt idx="76">
+                  <c:v>1.0002200000000001</c:v>
+                </c:pt>
+                <c:pt idx="77">
+                  <c:v>1.00021</c:v>
+                </c:pt>
+                <c:pt idx="78">
+                  <c:v>1.0002</c:v>
+                </c:pt>
+                <c:pt idx="79">
+                  <c:v>1.0001800000000001</c:v>
+                </c:pt>
+                <c:pt idx="80">
+                  <c:v>1.00017</c:v>
+                </c:pt>
+                <c:pt idx="81">
+                  <c:v>1.0001599999999999</c:v>
+                </c:pt>
+                <c:pt idx="82">
+                  <c:v>1.0001500000000001</c:v>
+                </c:pt>
+                <c:pt idx="83">
+                  <c:v>1.00014</c:v>
+                </c:pt>
+                <c:pt idx="84">
+                  <c:v>1.00013</c:v>
+                </c:pt>
+                <c:pt idx="85">
+                  <c:v>1.0001199999999999</c:v>
+                </c:pt>
+                <c:pt idx="86">
+                  <c:v>1.0001100000000001</c:v>
+                </c:pt>
+                <c:pt idx="87">
+                  <c:v>1.0001</c:v>
+                </c:pt>
+                <c:pt idx="88">
+                  <c:v>1.0001</c:v>
+                </c:pt>
+                <c:pt idx="89">
+                  <c:v>1.0000899999999999</c:v>
+                </c:pt>
+                <c:pt idx="90">
+                  <c:v>1.0000800000000001</c:v>
+                </c:pt>
+                <c:pt idx="91">
+                  <c:v>1.0000800000000001</c:v>
+                </c:pt>
+                <c:pt idx="92">
+                  <c:v>1.00007</c:v>
+                </c:pt>
+                <c:pt idx="93">
+                  <c:v>1.0000599999999999</c:v>
+                </c:pt>
+                <c:pt idx="94">
+                  <c:v>1.0000599999999999</c:v>
+                </c:pt>
+                <c:pt idx="95">
+                  <c:v>1.0000500000000001</c:v>
+                </c:pt>
+                <c:pt idx="96">
+                  <c:v>1.0000500000000001</c:v>
+                </c:pt>
+                <c:pt idx="97">
+                  <c:v>1.0000500000000001</c:v>
+                </c:pt>
+                <c:pt idx="98">
+                  <c:v>1.00004</c:v>
+                </c:pt>
+                <c:pt idx="99">
+                  <c:v>1.00004</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="-1486007888"/>
+        <c:axId val="-1486003536"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="-1486007888"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="-1486003536"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="-1486003536"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="-1486007888"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -1977,11 +2876,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="57706816"/>
-        <c:axId val="57702464"/>
+        <c:axId val="-1486005168"/>
+        <c:axId val="-1486002992"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="57706816"/>
+        <c:axId val="-1486005168"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2038,12 +2937,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="57702464"/>
+        <c:crossAx val="-1486002992"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="57702464"/>
+        <c:axId val="-1486002992"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2100,7 +2999,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="57706816"/>
+        <c:crossAx val="-1486005168"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2181,7 +3080,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -3581,11 +4480,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="250517008"/>
-        <c:axId val="250516464"/>
+        <c:axId val="-1559880672"/>
+        <c:axId val="-1559887200"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="250517008"/>
+        <c:axId val="-1559880672"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3642,12 +4541,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="250516464"/>
+        <c:crossAx val="-1559887200"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="250516464"/>
+        <c:axId val="-1559887200"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3704,7 +4603,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="250517008"/>
+        <c:crossAx val="-1559880672"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3865,6 +4764,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
@@ -4897,20 +5836,536 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>175260</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>144780</xdr:rowOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>7620</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>7620</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>18</xdr:col>
-      <xdr:colOff>480060</xdr:colOff>
-      <xdr:row>15</xdr:row>
-      <xdr:rowOff>144780</xdr:rowOff>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>312420</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>7620</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -4931,16 +6386,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>175260</xdr:colOff>
-      <xdr:row>15</xdr:row>
-      <xdr:rowOff>175260</xdr:rowOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>167640</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>18</xdr:col>
-      <xdr:colOff>480060</xdr:colOff>
-      <xdr:row>30</xdr:row>
-      <xdr:rowOff>175260</xdr:rowOff>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>304800</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>167640</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -4954,6 +6409,36 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>308610</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>160020</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>3810</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>160020</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="Chart 3"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -5225,15 +6710,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E101"/>
+  <dimension ref="A1:S101"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I21" sqref="I21"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="P20" sqref="P20:S23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -5249,8 +6734,11 @@
       <c r="E1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>0</v>
       </c>
@@ -5266,8 +6754,11 @@
       <c r="E2">
         <v>10</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F2">
+        <v>2.0400299999999998</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>1</v>
       </c>
@@ -5283,8 +6774,11 @@
       <c r="E3">
         <v>10</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F3">
+        <v>1.4293100000000001</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>2</v>
       </c>
@@ -5300,8 +6794,11 @@
       <c r="E4">
         <v>10</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F4">
+        <v>1.1956199999999999</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>3</v>
       </c>
@@ -5317,8 +6814,11 @@
       <c r="E5">
         <v>10</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F5">
+        <v>1.09382</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>4</v>
       </c>
@@ -5334,8 +6834,11 @@
       <c r="E6">
         <v>10</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F6">
+        <v>1.0470900000000001</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>5</v>
       </c>
@@ -5351,8 +6854,11 @@
       <c r="E7">
         <v>10</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F7">
+        <v>1.0262100000000001</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>6</v>
       </c>
@@ -5368,8 +6874,11 @@
       <c r="E8">
         <v>10</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F8">
+        <v>1.0192399999999999</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>7</v>
       </c>
@@ -5385,8 +6894,11 @@
       <c r="E9">
         <v>10</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F9">
+        <v>1.0223899999999999</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>8</v>
       </c>
@@ -5402,8 +6914,11 @@
       <c r="E10">
         <v>10</v>
       </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F10">
+        <v>1.0381400000000001</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>9</v>
       </c>
@@ -5419,8 +6934,11 @@
       <c r="E11">
         <v>10</v>
       </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F11">
+        <v>1.07914</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>10</v>
       </c>
@@ -5436,8 +6954,11 @@
       <c r="E12">
         <v>10</v>
       </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F12">
+        <v>1.18232</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>11</v>
       </c>
@@ -5453,8 +6974,11 @@
       <c r="E13">
         <v>10</v>
       </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F13">
+        <v>1.4361600000000001</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>12</v>
       </c>
@@ -5470,8 +6994,11 @@
       <c r="E14">
         <v>10</v>
       </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F14">
+        <v>1.9472100000000001</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>13</v>
       </c>
@@ -5487,8 +7014,11 @@
       <c r="E15">
         <v>10</v>
       </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F15">
+        <v>2.3772600000000002</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>14</v>
       </c>
@@ -5504,8 +7034,11 @@
       <c r="E16">
         <v>10</v>
       </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F16">
+        <v>1.7273400000000001</v>
+      </c>
+    </row>
+    <row r="17" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>15</v>
       </c>
@@ -5521,8 +7054,11 @@
       <c r="E17">
         <v>10</v>
       </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F17">
+        <v>1.45112</v>
+      </c>
+    </row>
+    <row r="18" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>16</v>
       </c>
@@ -5538,8 +7074,11 @@
       <c r="E18">
         <v>10</v>
       </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F18">
+        <v>1.6919</v>
+      </c>
+    </row>
+    <row r="19" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>17</v>
       </c>
@@ -5555,8 +7094,11 @@
       <c r="E19">
         <v>10</v>
       </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F19">
+        <v>1.9096599999999999</v>
+      </c>
+    </row>
+    <row r="20" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>18</v>
       </c>
@@ -5572,8 +7114,17 @@
       <c r="E20">
         <v>10</v>
       </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F20">
+        <v>1.5149999999999999</v>
+      </c>
+      <c r="P20" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="Q20" s="1"/>
+      <c r="R20" s="1"/>
+      <c r="S20" s="1"/>
+    </row>
+    <row r="21" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>19</v>
       </c>
@@ -5589,8 +7140,21 @@
       <c r="E21">
         <v>10</v>
       </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F21">
+        <v>3.6111800000000001</v>
+      </c>
+      <c r="P21" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="Q21" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="R21" s="1">
+        <v>0</v>
+      </c>
+      <c r="S21" s="1"/>
+    </row>
+    <row r="22" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>20</v>
       </c>
@@ -5606,8 +7170,19 @@
       <c r="E22">
         <v>10</v>
       </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F22">
+        <v>3.2484299999999999</v>
+      </c>
+      <c r="P22" s="1"/>
+      <c r="Q22" s="1">
+        <v>0</v>
+      </c>
+      <c r="R22" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="S22" s="1"/>
+    </row>
+    <row r="23" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>21</v>
       </c>
@@ -5623,8 +7198,15 @@
       <c r="E23">
         <v>10</v>
       </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F23">
+        <v>1.81172</v>
+      </c>
+      <c r="P23" s="1"/>
+      <c r="Q23" s="1"/>
+      <c r="R23" s="1"/>
+      <c r="S23" s="1"/>
+    </row>
+    <row r="24" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>22</v>
       </c>
@@ -5640,8 +7222,11 @@
       <c r="E24">
         <v>10</v>
       </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F24">
+        <v>1.36181</v>
+      </c>
+    </row>
+    <row r="25" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>23</v>
       </c>
@@ -5657,8 +7242,11 @@
       <c r="E25">
         <v>10</v>
       </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F25">
+        <v>1.19096</v>
+      </c>
+    </row>
+    <row r="26" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>24</v>
       </c>
@@ -5674,8 +7262,11 @@
       <c r="E26">
         <v>10</v>
       </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F26">
+        <v>1.1247499999999999</v>
+      </c>
+    </row>
+    <row r="27" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>25</v>
       </c>
@@ -5691,8 +7282,11 @@
       <c r="E27">
         <v>10</v>
       </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F27">
+        <v>1.10076</v>
+      </c>
+    </row>
+    <row r="28" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>26</v>
       </c>
@@ -5708,8 +7302,11 @@
       <c r="E28">
         <v>10</v>
       </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F28">
+        <v>1.08213</v>
+      </c>
+    </row>
+    <row r="29" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>27</v>
       </c>
@@ -5725,8 +7322,11 @@
       <c r="E29">
         <v>10</v>
       </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F29">
+        <v>1.04671</v>
+      </c>
+    </row>
+    <row r="30" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>28</v>
       </c>
@@ -5742,8 +7342,11 @@
       <c r="E30">
         <v>10</v>
       </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F30">
+        <v>1.0276000000000001</v>
+      </c>
+    </row>
+    <row r="31" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>29</v>
       </c>
@@ -5759,8 +7362,11 @@
       <c r="E31">
         <v>10</v>
       </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F31">
+        <v>1.0188299999999999</v>
+      </c>
+    </row>
+    <row r="32" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A32">
         <v>30</v>
       </c>
@@ -5776,8 +7382,11 @@
       <c r="E32">
         <v>10</v>
       </c>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F32">
+        <v>1.0133399999999999</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A33">
         <v>31</v>
       </c>
@@ -5793,8 +7402,11 @@
       <c r="E33">
         <v>10</v>
       </c>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F33">
+        <v>1.0102599999999999</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A34">
         <v>32</v>
       </c>
@@ -5810,8 +7422,11 @@
       <c r="E34">
         <v>10</v>
       </c>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F34">
+        <v>1.00824</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A35">
         <v>33</v>
       </c>
@@ -5827,8 +7442,11 @@
       <c r="E35">
         <v>10</v>
       </c>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F35">
+        <v>1.00688</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A36">
         <v>34</v>
       </c>
@@ -5844,8 +7462,11 @@
       <c r="E36">
         <v>10</v>
       </c>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F36">
+        <v>1.00589</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A37">
         <v>35</v>
       </c>
@@ -5861,8 +7482,11 @@
       <c r="E37">
         <v>10</v>
       </c>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F37">
+        <v>1.0051399999999999</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A38">
         <v>36</v>
       </c>
@@ -5878,8 +7502,11 @@
       <c r="E38">
         <v>10</v>
       </c>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F38">
+        <v>1.0045299999999999</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A39">
         <v>37</v>
       </c>
@@ -5895,8 +7522,11 @@
       <c r="E39">
         <v>10</v>
       </c>
-    </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F39">
+        <v>1.00404</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A40">
         <v>38</v>
       </c>
@@ -5912,8 +7542,11 @@
       <c r="E40">
         <v>10</v>
       </c>
-    </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F40">
+        <v>1.00362</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A41">
         <v>39</v>
       </c>
@@ -5929,8 +7562,11 @@
       <c r="E41">
         <v>10</v>
       </c>
-    </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F41">
+        <v>1.00326</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A42">
         <v>40</v>
       </c>
@@ -5946,8 +7582,11 @@
       <c r="E42">
         <v>10</v>
       </c>
-    </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F42">
+        <v>1.00295</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A43">
         <v>41</v>
       </c>
@@ -5963,8 +7602,11 @@
       <c r="E43">
         <v>10</v>
       </c>
-    </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F43">
+        <v>1.00268</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A44">
         <v>42</v>
       </c>
@@ -5980,8 +7622,11 @@
       <c r="E44">
         <v>10</v>
       </c>
-    </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F44">
+        <v>1.00244</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A45">
         <v>43</v>
       </c>
@@ -5997,8 +7642,11 @@
       <c r="E45">
         <v>10</v>
       </c>
-    </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F45">
+        <v>1.00223</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A46">
         <v>44</v>
       </c>
@@ -6014,8 +7662,11 @@
       <c r="E46">
         <v>10</v>
       </c>
-    </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F46">
+        <v>1.0020500000000001</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A47">
         <v>45</v>
       </c>
@@ -6031,8 +7682,11 @@
       <c r="E47">
         <v>10</v>
       </c>
-    </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F47">
+        <v>1.0018800000000001</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A48">
         <v>46</v>
       </c>
@@ -6048,8 +7702,11 @@
       <c r="E48">
         <v>10</v>
       </c>
-    </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F48">
+        <v>1.00173</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A49">
         <v>47</v>
       </c>
@@ -6065,8 +7722,11 @@
       <c r="E49">
         <v>10</v>
       </c>
-    </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F49">
+        <v>1.0016</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A50">
         <v>48</v>
       </c>
@@ -6082,8 +7742,11 @@
       <c r="E50">
         <v>10</v>
       </c>
-    </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F50">
+        <v>1.0014799999999999</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A51">
         <v>49</v>
       </c>
@@ -6099,8 +7762,11 @@
       <c r="E51">
         <v>10</v>
       </c>
-    </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F51">
+        <v>1.0013700000000001</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A52">
         <v>50</v>
       </c>
@@ -6116,8 +7782,11 @@
       <c r="E52">
         <v>10</v>
       </c>
-    </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F52">
+        <v>1.0012700000000001</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A53">
         <v>51</v>
       </c>
@@ -6133,8 +7802,11 @@
       <c r="E53">
         <v>10</v>
       </c>
-    </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F53">
+        <v>1.0011699999999999</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A54">
         <v>52</v>
       </c>
@@ -6150,8 +7822,11 @@
       <c r="E54">
         <v>10</v>
       </c>
-    </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F54">
+        <v>1.00109</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A55">
         <v>53</v>
       </c>
@@ -6167,8 +7842,11 @@
       <c r="E55">
         <v>10</v>
       </c>
-    </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F55">
+        <v>1.00101</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A56">
         <v>54</v>
       </c>
@@ -6184,8 +7862,11 @@
       <c r="E56">
         <v>10</v>
       </c>
-    </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F56">
+        <v>1.00095</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A57">
         <v>55</v>
       </c>
@@ -6201,8 +7882,11 @@
       <c r="E57">
         <v>10</v>
       </c>
-    </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F57">
+        <v>1.00088</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A58">
         <v>56</v>
       </c>
@@ -6218,8 +7902,11 @@
       <c r="E58">
         <v>10</v>
       </c>
-    </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F58">
+        <v>1.00082</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A59">
         <v>57</v>
       </c>
@@ -6235,8 +7922,11 @@
       <c r="E59">
         <v>10</v>
       </c>
-    </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F59">
+        <v>1.0007699999999999</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A60">
         <v>58</v>
       </c>
@@ -6252,8 +7942,11 @@
       <c r="E60">
         <v>10</v>
       </c>
-    </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F60">
+        <v>1.0007200000000001</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A61">
         <v>59</v>
       </c>
@@ -6269,8 +7962,11 @@
       <c r="E61">
         <v>10</v>
       </c>
-    </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F61">
+        <v>1.0006699999999999</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A62">
         <v>60</v>
       </c>
@@ -6286,8 +7982,11 @@
       <c r="E62">
         <v>10</v>
       </c>
-    </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F62">
+        <v>1.0006299999999999</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A63">
         <v>61</v>
       </c>
@@ -6303,8 +8002,11 @@
       <c r="E63">
         <v>10</v>
       </c>
-    </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F63">
+        <v>1.0005900000000001</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A64">
         <v>62</v>
       </c>
@@ -6320,8 +8022,11 @@
       <c r="E64">
         <v>10</v>
       </c>
-    </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F64">
+        <v>1.0005500000000001</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A65">
         <v>63</v>
       </c>
@@ -6337,8 +8042,11 @@
       <c r="E65">
         <v>10</v>
       </c>
-    </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F65">
+        <v>1.0005200000000001</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A66">
         <v>64</v>
       </c>
@@ -6354,8 +8062,11 @@
       <c r="E66">
         <v>10</v>
       </c>
-    </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F66">
+        <v>1.00048</v>
+      </c>
+    </row>
+    <row r="67" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A67">
         <v>65</v>
       </c>
@@ -6371,8 +8082,11 @@
       <c r="E67">
         <v>10</v>
       </c>
-    </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F67">
+        <v>1.0004500000000001</v>
+      </c>
+    </row>
+    <row r="68" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A68">
         <v>66</v>
       </c>
@@ -6388,8 +8102,11 @@
       <c r="E68">
         <v>10</v>
       </c>
-    </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F68">
+        <v>1.0004200000000001</v>
+      </c>
+    </row>
+    <row r="69" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A69">
         <v>67</v>
       </c>
@@ -6405,8 +8122,11 @@
       <c r="E69">
         <v>10</v>
       </c>
-    </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F69">
+        <v>1.0004</v>
+      </c>
+    </row>
+    <row r="70" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A70">
         <v>68</v>
       </c>
@@ -6422,8 +8142,11 @@
       <c r="E70">
         <v>10</v>
       </c>
-    </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F70">
+        <v>1.00037</v>
+      </c>
+    </row>
+    <row r="71" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A71">
         <v>69</v>
       </c>
@@ -6439,8 +8162,11 @@
       <c r="E71">
         <v>10</v>
       </c>
-    </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F71">
+        <v>1.0003500000000001</v>
+      </c>
+    </row>
+    <row r="72" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A72">
         <v>70</v>
       </c>
@@ -6456,8 +8182,11 @@
       <c r="E72">
         <v>10</v>
       </c>
-    </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F72">
+        <v>1.0003299999999999</v>
+      </c>
+    </row>
+    <row r="73" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A73">
         <v>71</v>
       </c>
@@ -6473,8 +8202,11 @@
       <c r="E73">
         <v>10</v>
       </c>
-    </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F73">
+        <v>1.00031</v>
+      </c>
+    </row>
+    <row r="74" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A74">
         <v>72</v>
       </c>
@@ -6490,8 +8222,11 @@
       <c r="E74">
         <v>10</v>
       </c>
-    </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F74">
+        <v>1.0002899999999999</v>
+      </c>
+    </row>
+    <row r="75" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A75">
         <v>73</v>
       </c>
@@ -6507,8 +8242,11 @@
       <c r="E75">
         <v>10</v>
       </c>
-    </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F75">
+        <v>1.00027</v>
+      </c>
+    </row>
+    <row r="76" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A76">
         <v>74</v>
       </c>
@@ -6524,8 +8262,11 @@
       <c r="E76">
         <v>10</v>
       </c>
-    </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F76">
+        <v>1.0002500000000001</v>
+      </c>
+    </row>
+    <row r="77" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A77">
         <v>75</v>
       </c>
@@ -6541,8 +8282,11 @@
       <c r="E77">
         <v>10</v>
       </c>
-    </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F77">
+        <v>1.00024</v>
+      </c>
+    </row>
+    <row r="78" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A78">
         <v>76</v>
       </c>
@@ -6558,8 +8302,11 @@
       <c r="E78">
         <v>10</v>
       </c>
-    </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F78">
+        <v>1.0002200000000001</v>
+      </c>
+    </row>
+    <row r="79" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A79">
         <v>77</v>
       </c>
@@ -6575,8 +8322,11 @@
       <c r="E79">
         <v>10</v>
       </c>
-    </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F79">
+        <v>1.00021</v>
+      </c>
+    </row>
+    <row r="80" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A80">
         <v>78</v>
       </c>
@@ -6592,8 +8342,11 @@
       <c r="E80">
         <v>10</v>
       </c>
-    </row>
-    <row r="81" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F80">
+        <v>1.0002</v>
+      </c>
+    </row>
+    <row r="81" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A81">
         <v>79</v>
       </c>
@@ -6609,8 +8362,11 @@
       <c r="E81">
         <v>10</v>
       </c>
-    </row>
-    <row r="82" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F81">
+        <v>1.0001800000000001</v>
+      </c>
+    </row>
+    <row r="82" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A82">
         <v>80</v>
       </c>
@@ -6626,8 +8382,11 @@
       <c r="E82">
         <v>10</v>
       </c>
-    </row>
-    <row r="83" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F82">
+        <v>1.00017</v>
+      </c>
+    </row>
+    <row r="83" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A83">
         <v>81</v>
       </c>
@@ -6643,8 +8402,11 @@
       <c r="E83">
         <v>10</v>
       </c>
-    </row>
-    <row r="84" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F83">
+        <v>1.0001599999999999</v>
+      </c>
+    </row>
+    <row r="84" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A84">
         <v>82</v>
       </c>
@@ -6660,8 +8422,11 @@
       <c r="E84">
         <v>10</v>
       </c>
-    </row>
-    <row r="85" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F84">
+        <v>1.0001500000000001</v>
+      </c>
+    </row>
+    <row r="85" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A85">
         <v>83</v>
       </c>
@@ -6677,8 +8442,11 @@
       <c r="E85">
         <v>10</v>
       </c>
-    </row>
-    <row r="86" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F85">
+        <v>1.00014</v>
+      </c>
+    </row>
+    <row r="86" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A86">
         <v>84</v>
       </c>
@@ -6694,8 +8462,11 @@
       <c r="E86">
         <v>10</v>
       </c>
-    </row>
-    <row r="87" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F86">
+        <v>1.00013</v>
+      </c>
+    </row>
+    <row r="87" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A87">
         <v>85</v>
       </c>
@@ -6711,8 +8482,11 @@
       <c r="E87">
         <v>10</v>
       </c>
-    </row>
-    <row r="88" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F87">
+        <v>1.0001199999999999</v>
+      </c>
+    </row>
+    <row r="88" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A88">
         <v>86</v>
       </c>
@@ -6728,8 +8502,11 @@
       <c r="E88">
         <v>10</v>
       </c>
-    </row>
-    <row r="89" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F88">
+        <v>1.0001100000000001</v>
+      </c>
+    </row>
+    <row r="89" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A89">
         <v>87</v>
       </c>
@@ -6745,8 +8522,11 @@
       <c r="E89">
         <v>10</v>
       </c>
-    </row>
-    <row r="90" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F89">
+        <v>1.0001</v>
+      </c>
+    </row>
+    <row r="90" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A90">
         <v>88</v>
       </c>
@@ -6762,8 +8542,11 @@
       <c r="E90">
         <v>10</v>
       </c>
-    </row>
-    <row r="91" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F90">
+        <v>1.0001</v>
+      </c>
+    </row>
+    <row r="91" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A91">
         <v>89</v>
       </c>
@@ -6779,8 +8562,11 @@
       <c r="E91">
         <v>10</v>
       </c>
-    </row>
-    <row r="92" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F91">
+        <v>1.0000899999999999</v>
+      </c>
+    </row>
+    <row r="92" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A92">
         <v>90</v>
       </c>
@@ -6796,8 +8582,11 @@
       <c r="E92">
         <v>10</v>
       </c>
-    </row>
-    <row r="93" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F92">
+        <v>1.0000800000000001</v>
+      </c>
+    </row>
+    <row r="93" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A93">
         <v>91</v>
       </c>
@@ -6813,8 +8602,11 @@
       <c r="E93">
         <v>10</v>
       </c>
-    </row>
-    <row r="94" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F93">
+        <v>1.0000800000000001</v>
+      </c>
+    </row>
+    <row r="94" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A94">
         <v>92</v>
       </c>
@@ -6830,8 +8622,11 @@
       <c r="E94">
         <v>10</v>
       </c>
-    </row>
-    <row r="95" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F94">
+        <v>1.00007</v>
+      </c>
+    </row>
+    <row r="95" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A95">
         <v>93</v>
       </c>
@@ -6847,8 +8642,11 @@
       <c r="E95">
         <v>10</v>
       </c>
-    </row>
-    <row r="96" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F95">
+        <v>1.0000599999999999</v>
+      </c>
+    </row>
+    <row r="96" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A96">
         <v>94</v>
       </c>
@@ -6864,8 +8662,11 @@
       <c r="E96">
         <v>10</v>
       </c>
-    </row>
-    <row r="97" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F96">
+        <v>1.0000599999999999</v>
+      </c>
+    </row>
+    <row r="97" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A97">
         <v>95</v>
       </c>
@@ -6881,8 +8682,11 @@
       <c r="E97">
         <v>10</v>
       </c>
-    </row>
-    <row r="98" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F97">
+        <v>1.0000500000000001</v>
+      </c>
+    </row>
+    <row r="98" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A98">
         <v>96</v>
       </c>
@@ -6898,8 +8702,11 @@
       <c r="E98">
         <v>10</v>
       </c>
-    </row>
-    <row r="99" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F98">
+        <v>1.0000500000000001</v>
+      </c>
+    </row>
+    <row r="99" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A99">
         <v>97</v>
       </c>
@@ -6915,8 +8722,11 @@
       <c r="E99">
         <v>10</v>
       </c>
-    </row>
-    <row r="100" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F99">
+        <v>1.0000500000000001</v>
+      </c>
+    </row>
+    <row r="100" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A100">
         <v>98</v>
       </c>
@@ -6932,8 +8742,11 @@
       <c r="E100">
         <v>10</v>
       </c>
-    </row>
-    <row r="101" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F100">
+        <v>1.00004</v>
+      </c>
+    </row>
+    <row r="101" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A101">
         <v>99</v>
       </c>
@@ -6948,6 +8761,9 @@
       </c>
       <c r="E101">
         <v>10</v>
+      </c>
+      <c r="F101">
+        <v>1.00004</v>
       </c>
     </row>
   </sheetData>

</xml_diff>